<commit_message>
update to login page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 LoginPage.xlsx
+++ b/Testing Spreadsheet v1.0 LoginPage.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="25400" windowHeight="16020" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="25400" windowHeight="16020" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="183">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -421,18 +421,6 @@
     <t>Login_Tproc_1</t>
   </si>
   <si>
-    <t>While on the login page enter valid username and password and click login</t>
-  </si>
-  <si>
-    <t>The user is logged in</t>
-  </si>
-  <si>
-    <t>automated selenium test</t>
-  </si>
-  <si>
-    <t>Login_</t>
-  </si>
-  <si>
     <t>Login_TConn_2</t>
   </si>
   <si>
@@ -556,9 +544,6 @@
     <t>To show that if the user is not logged in and tries to navigate to the order page the user is directed to login</t>
   </si>
   <si>
-    <t>To show that from any web page the user can navigate to the login page</t>
-  </si>
-  <si>
     <t>To show that the user can navigate to the forgot password page from the login page</t>
   </si>
   <si>
@@ -592,9 +577,6 @@
     <t>To show that when the user clicks the register page that the user is taken to the appropriate page</t>
   </si>
   <si>
-    <t>To show the system prevents unregistered and registered but not logged in users from accessing registered parts of the site</t>
-  </si>
-  <si>
     <t>3.2.1</t>
   </si>
   <si>
@@ -628,24 +610,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Login_TConn_24</t>
-  </si>
-  <si>
-    <t>Login_TConn_25</t>
-  </si>
-  <si>
-    <t>Login_TConn_26</t>
-  </si>
-  <si>
-    <t>Login_TConn_27</t>
-  </si>
-  <si>
-    <t>Login_TConn_28</t>
-  </si>
-  <si>
-    <t>Login_TConn_29</t>
-  </si>
-  <si>
     <t>Chris McClune</t>
   </si>
   <si>
@@ -718,35 +682,116 @@
     <t>Login_TCase_24</t>
   </si>
   <si>
-    <t>Login_TCase_25</t>
-  </si>
-  <si>
-    <t>Login_TCase_26</t>
-  </si>
-  <si>
-    <t>Login_TCase_27</t>
-  </si>
-  <si>
-    <t>Login_TCase_28</t>
-  </si>
-  <si>
-    <t>Login_TCase_29</t>
-  </si>
-  <si>
-    <t>Login_TCase_30</t>
-  </si>
-  <si>
-    <t>Login_TCase_31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check </t>
+    <t>Check that the footer on the login page shows the copyright and version information</t>
+  </si>
+  <si>
+    <t>Check if the login page has appropriate validation as there is user input required</t>
+  </si>
+  <si>
+    <t>email: cmcclune02@qub.ac.uk password: validPassword</t>
+  </si>
+  <si>
+    <t>Check that the login page has a title</t>
+  </si>
+  <si>
+    <t>Check that the systerm has a functional login page</t>
+  </si>
+  <si>
+    <t>Be on the home page and click login page</t>
+  </si>
+  <si>
+    <t>Check that the login page has a common navigation area</t>
+  </si>
+  <si>
+    <t>Check that if the user is not logged in and tried to navigate to the order page the user is directed to the login page</t>
+  </si>
+  <si>
+    <t>not be logged in</t>
+  </si>
+  <si>
+    <t>To show that from any web page the user can navigate to the login page if they are not logged in</t>
+  </si>
+  <si>
+    <t>Check that from any web page that the user can navigate to the login page if they are not logged in</t>
+  </si>
+  <si>
+    <t>Check that a user can navigate to the forgot password page from the login page</t>
+  </si>
+  <si>
+    <t>Check that a registered user can login to the system using a valid username and password</t>
+  </si>
+  <si>
+    <t>Check that a non registered user cannot login to the system without a valid username and password</t>
+  </si>
+  <si>
+    <t>email: cmcclune02@qub.ac.uk password: invalidPassword</t>
+  </si>
+  <si>
+    <t>Check that a valid username is in email address format and a valid password is at least 6 characters</t>
+  </si>
+  <si>
+    <t>Check that the login page has links to the forgot password and register pages</t>
+  </si>
+  <si>
+    <t>Check that when the user clicks the forgot password link that they are taken to the correct page</t>
+  </si>
+  <si>
+    <t>Check that when the user clicks the register link that they are taken to the correct page</t>
+  </si>
+  <si>
+    <t>To show the system prevents unregistered and registered but not logged in users from accessing restricted parts of the site</t>
+  </si>
+  <si>
+    <t>Check if unregistered and registered but not logged in users cannot access restricted parts of the system</t>
+  </si>
+  <si>
+    <t>URL's copied for each restricted page and used when not logged in</t>
+  </si>
+  <si>
+    <t>Check that the login page can be accessed using the target mobile devices</t>
+  </si>
+  <si>
+    <t>not be on login page, use target mobile devices</t>
+  </si>
+  <si>
+    <t>Check that the login page can be accessed using the target web browsers</t>
+  </si>
+  <si>
+    <t>Check that the layout of the login page is consistent with the other pages</t>
+  </si>
+  <si>
+    <t>all other web pages in system</t>
+  </si>
+  <si>
+    <t>Check that the login page has no spelling or grammatical errors</t>
+  </si>
+  <si>
+    <t>Check to see if the remember me button remembers details of the previouis user</t>
+  </si>
+  <si>
+    <t>Be on the login page. Have the remember me button selected</t>
+  </si>
+  <si>
+    <t>Defect_login_1</t>
+  </si>
+  <si>
+    <t>The validation message does not show on screen. It appears that a post back occurs to the server. Would recommend that this is prevented by catching the validation error on the clients browser.</t>
+  </si>
+  <si>
+    <t>Check user is blocked from logging in with an invalid email address but a valid password</t>
+  </si>
+  <si>
+    <t>email: cmcclune02qub.ac.uk password: validPassword</t>
+  </si>
+  <si>
+    <t>Check user is blocked from logging in with an valid email address but a invalid password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -854,6 +899,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -939,9 +990,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -977,9 +1032,6 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1045,11 +1097,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1145,7 +1204,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Cases'!$T$8:$T$10</c:f>
+              <c:f>'Test Cases'!$T$10:$T$12</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1162,15 +1221,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Cases'!$U$8:$U$10</c:f>
+              <c:f>'Test Cases'!$U$10:$U$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1235,7 +1294,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Cases'!$T$26:$T$30</c:f>
+              <c:f>'Test Cases'!$T$28:$T$32</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1258,7 +1317,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Cases'!$U$26:$U$30</c:f>
+              <c:f>'Test Cases'!$U$28:$U$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1266,7 +1325,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1290,11 +1349,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2135327784"/>
-        <c:axId val="2135320472"/>
+        <c:axId val="2134575352"/>
+        <c:axId val="2137094952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2135327784"/>
+        <c:axId val="2134575352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1362,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135320472"/>
+        <c:crossAx val="2137094952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1311,7 +1370,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135320472"/>
+        <c:axId val="2137094952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1381,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135327784"/>
+        <c:crossAx val="2134575352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1345,13 +1404,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>46567</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>351367</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1375,13 +1434,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>21166</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>325966</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1735,8 +1794,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1748,16 +1807,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25" customHeight="1">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="27" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1766,127 +1825,127 @@
         <v>59</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="35.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="31"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="28">
       <c r="A4" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="23">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="31" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="23">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="23">
       <c r="A7" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="32" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="28">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="33" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>6</v>
@@ -1894,13 +1953,13 @@
     </row>
     <row r="10" spans="1:9" ht="28">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>6</v>
@@ -1908,13 +1967,13 @@
     </row>
     <row r="11" spans="1:9" ht="28">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>6</v>
@@ -1922,13 +1981,13 @@
     </row>
     <row r="12" spans="1:9" ht="28">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>6</v>
@@ -1936,13 +1995,13 @@
     </row>
     <row r="13" spans="1:9" ht="28">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>6</v>
@@ -1950,13 +2009,13 @@
     </row>
     <row r="14" spans="1:9" ht="42">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>6</v>
@@ -1964,13 +2023,13 @@
     </row>
     <row r="15" spans="1:9" ht="28">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
@@ -1978,13 +2037,13 @@
     </row>
     <row r="16" spans="1:9" ht="28">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
@@ -1992,13 +2051,13 @@
     </row>
     <row r="17" spans="1:4" ht="28">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>27</v>
@@ -2006,13 +2065,13 @@
     </row>
     <row r="18" spans="1:4" ht="28">
       <c r="A18" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>6</v>
@@ -2020,13 +2079,13 @@
     </row>
     <row r="19" spans="1:4" ht="28">
       <c r="A19" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>27</v>
@@ -2034,13 +2093,13 @@
     </row>
     <row r="20" spans="1:4" ht="28">
       <c r="A20" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
@@ -2048,13 +2107,13 @@
     </row>
     <row r="21" spans="1:4" ht="28">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>11</v>
@@ -2062,13 +2121,13 @@
     </row>
     <row r="22" spans="1:4" ht="28">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>11</v>
@@ -2076,13 +2135,13 @@
     </row>
     <row r="23" spans="1:4" ht="42">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>11</v>
@@ -2090,13 +2149,13 @@
     </row>
     <row r="24" spans="1:4" ht="28">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>11</v>
@@ -2129,16 +2188,16 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:Z161"/>
+  <dimension ref="A1:Z163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
     <col min="4" max="4" width="32.5" customWidth="1"/>
     <col min="5" max="6" width="18.5" customWidth="1"/>
@@ -2149,71 +2208,71 @@
     <col min="12" max="12" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="12.83203125" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="41.83203125" customWidth="1"/>
+    <col min="15" max="15" width="159.1640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.6640625" customWidth="1"/>
     <col min="20" max="20" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="17"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="26">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>129</v>
+        <v>122</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>59</v>
@@ -2224,11 +2283,11 @@
       <c r="G2" s="10">
         <v>42077</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="23" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -2241,21 +2300,34 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="23">
+    <row r="3" spans="1:26" ht="39">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+        <v>148</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="24"/>
+        <v>61</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -2263,93 +2335,161 @@
       <c r="N3" s="3"/>
       <c r="O3" s="6"/>
       <c r="P3" s="7"/>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="23">
+    <row r="4" spans="1:26" ht="26">
       <c r="A4" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>150</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="6"/>
+        <v>62</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="10">
+        <v>42077</v>
+      </c>
       <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="6" t="s">
+        <v>179</v>
+      </c>
       <c r="P4" s="7"/>
       <c r="Z4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" ht="39">
       <c r="A5" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>162</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="10"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="Z5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" ht="39">
       <c r="A6" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>181</v>
+      </c>
       <c r="E6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="10"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="7"/>
+      <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="11"/>
+        <v>63</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -2357,79 +2497,110 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="7"/>
-      <c r="T7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26">
+    </row>
+    <row r="8" spans="1:26" ht="26">
       <c r="A8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" s="6"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
       <c r="P8" s="7"/>
-      <c r="T8" t="s">
-        <v>53</v>
-      </c>
-      <c r="U8" s="29">
-        <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
+    </row>
+    <row r="9" spans="1:26" ht="26">
       <c r="A9" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="10">
+        <v>42077</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="6"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
       <c r="P9" s="7"/>
       <c r="T9" t="s">
-        <v>25</v>
-      </c>
-      <c r="U9" s="29">
-        <f>COUNTIF(H3:H90,"*Failed*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="42">
       <c r="A10" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J10" s="7"/>
       <c r="K10" s="4"/>
       <c r="L10" s="7"/>
@@ -2438,24 +2609,41 @@
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="T10" t="s">
-        <v>54</v>
-      </c>
-      <c r="U10" s="29">
-        <f>COUNTIF(H4:H90,"*Not*")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26">
+        <v>53</v>
+      </c>
+      <c r="U10" s="28">
+        <f>COUNTIF(H2:H92,"*Passed*")</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="42">
       <c r="A11" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="7"/>
+        <v>67</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J11" s="7"/>
       <c r="K11" s="4"/>
       <c r="L11" s="7"/>
@@ -2463,56 +2651,121 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="T11" t="s">
+        <v>25</v>
+      </c>
+      <c r="U11" s="28">
+        <f>COUNTIF(H3:H92,"*Failed*")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="39">
       <c r="A12" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="7"/>
+        <v>68</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="K12" s="4"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="T12" t="s">
+        <v>54</v>
+      </c>
+      <c r="U12" s="28">
+        <f>COUNTIF(H4:H92,"*Not*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="39">
       <c r="A13" s="3" t="s">
-        <v>147</v>
+        <v>135</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="7"/>
+        <v>69</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
     </row>
-    <row r="14" spans="1:26">
+    <row r="14" spans="1:26" ht="39">
       <c r="A14" s="3" t="s">
-        <v>148</v>
+        <v>136</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
@@ -2521,17 +2774,34 @@
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" ht="39">
       <c r="A15" s="3" t="s">
-        <v>149</v>
+        <v>137</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="7"/>
+        <v>71</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -2540,17 +2810,34 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:26">
+    <row r="16" spans="1:26" ht="39">
       <c r="A16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>150</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="7"/>
+        <v>72</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -2559,17 +2846,34 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" ht="26">
       <c r="A17" s="3" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -2578,17 +2882,34 @@
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" ht="39">
       <c r="A18" s="3" t="s">
-        <v>152</v>
+        <v>140</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="7"/>
+        <v>74</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
@@ -2597,17 +2918,34 @@
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" ht="39">
       <c r="A19" s="3" t="s">
-        <v>153</v>
+        <v>141</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="7"/>
+        <v>75</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
@@ -2616,17 +2954,34 @@
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" ht="39">
       <c r="A20" s="3" t="s">
-        <v>154</v>
+        <v>142</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
@@ -2635,17 +2990,34 @@
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" ht="26">
       <c r="A21" s="3" t="s">
-        <v>155</v>
+        <v>143</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="7"/>
+        <v>77</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -2654,17 +3026,34 @@
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" ht="26">
       <c r="A22" s="3" t="s">
-        <v>156</v>
+        <v>144</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="7"/>
+        <v>78</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
@@ -2673,17 +3062,34 @@
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" ht="26">
       <c r="A23" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="7"/>
+        <v>79</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -2692,17 +3098,34 @@
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" ht="26">
       <c r="A24" s="3" t="s">
-        <v>158</v>
+        <v>146</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -2711,17 +3134,34 @@
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" ht="39">
       <c r="A25" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>150</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="35">
+        <v>42077</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -2729,21 +3169,14 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
-      <c r="T25" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>131</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="E26" s="1"/>
       <c r="F26" s="8"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="7"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="9"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
@@ -2751,25 +3184,14 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
-      <c r="T26" t="s">
-        <v>34</v>
-      </c>
-      <c r="U26" s="29">
-        <f>COUNTIF(L2:L50,"*Minor*")</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="27" spans="1:21">
-      <c r="A27" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>132</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="8"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="7"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="9"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -2778,23 +3200,15 @@
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
       <c r="T27" t="s">
-        <v>57</v>
-      </c>
-      <c r="U27" s="29">
-        <f>COUNTIF(L2:L7,"*Moderate*")</f>
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>133</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="E28" s="1"/>
       <c r="F28" s="8"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="23"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -2804,23 +3218,19 @@
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="T28" t="s">
-        <v>35</v>
-      </c>
-      <c r="U28" s="29">
-        <f>COUNTIF(L2:L7,"*Major*")</f>
+        <v>34</v>
+      </c>
+      <c r="U28" s="28">
+        <f>COUNTIF(L2:L52,"*Minor*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:21">
-      <c r="A29" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>134</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="E29" s="1"/>
       <c r="F29" s="8"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="23"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
@@ -2830,23 +3240,19 @@
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="T29" t="s">
-        <v>36</v>
-      </c>
-      <c r="U29" s="29">
-        <f>COUNTIF(L2:L7,"*Critical*")</f>
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="U29" s="28">
+        <f>COUNTIF(L2:L9,"*Moderate*")</f>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>135</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="8"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="23"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -2856,21 +3262,19 @@
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="T30" t="s">
-        <v>38</v>
-      </c>
-      <c r="U30" s="29">
-        <f>COUNTIF(L2:L7,"*Cometic*")</f>
+        <v>35</v>
+      </c>
+      <c r="U30" s="28">
+        <f>COUNTIF(L2:L9,"*Major*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:21">
-      <c r="A31" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="A31" s="3"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="8"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="23"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
@@ -2879,15 +3283,20 @@
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
+      <c r="T31" t="s">
+        <v>36</v>
+      </c>
+      <c r="U31" s="28">
+        <f>COUNTIF(L2:L9,"*Critical*")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:21">
-      <c r="A32" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E32" s="7"/>
+      <c r="A32" s="3"/>
+      <c r="E32" s="1"/>
       <c r="F32" s="8"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="23"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -2896,12 +3305,20 @@
       <c r="N32" s="7"/>
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
-    </row>
-    <row r="33" spans="5:16">
+      <c r="T32" t="s">
+        <v>38</v>
+      </c>
+      <c r="U32" s="28">
+        <f>COUNTIF(L2:L9,"*Cometic*")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="3"/>
       <c r="E33" s="7"/>
       <c r="F33" s="8"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="23"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
@@ -2911,11 +3328,12 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
     </row>
-    <row r="34" spans="5:16">
+    <row r="34" spans="1:16">
+      <c r="A34" s="3"/>
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="24"/>
+      <c r="H34" s="23"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
@@ -2925,11 +3343,11 @@
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
     </row>
-    <row r="35" spans="5:16">
+    <row r="35" spans="1:16">
       <c r="E35" s="7"/>
       <c r="F35" s="8"/>
       <c r="G35" s="7"/>
-      <c r="H35" s="24"/>
+      <c r="H35" s="23"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
@@ -2939,11 +3357,11 @@
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
     </row>
-    <row r="36" spans="5:16">
+    <row r="36" spans="1:16">
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
@@ -2953,11 +3371,11 @@
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
     </row>
-    <row r="37" spans="5:16">
+    <row r="37" spans="1:16">
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
       <c r="G37" s="7"/>
-      <c r="H37" s="24"/>
+      <c r="H37" s="23"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
@@ -2967,11 +3385,11 @@
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
     </row>
-    <row r="38" spans="5:16">
+    <row r="38" spans="1:16">
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
       <c r="G38" s="7"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="23"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
@@ -2981,11 +3399,11 @@
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
     </row>
-    <row r="39" spans="5:16">
+    <row r="39" spans="1:16">
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
       <c r="G39" s="7"/>
-      <c r="H39" s="24"/>
+      <c r="H39" s="23"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
@@ -2995,11 +3413,11 @@
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
     </row>
-    <row r="40" spans="5:16">
+    <row r="40" spans="1:16">
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
       <c r="G40" s="7"/>
-      <c r="H40" s="24"/>
+      <c r="H40" s="23"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
@@ -3009,11 +3427,11 @@
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
     </row>
-    <row r="41" spans="5:16">
+    <row r="41" spans="1:16">
       <c r="E41" s="7"/>
       <c r="F41" s="8"/>
       <c r="G41" s="7"/>
-      <c r="H41" s="24"/>
+      <c r="H41" s="23"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
@@ -3023,11 +3441,11 @@
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
     </row>
-    <row r="42" spans="5:16">
+    <row r="42" spans="1:16">
       <c r="E42" s="7"/>
       <c r="F42" s="8"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="24"/>
+      <c r="H42" s="23"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
@@ -3037,11 +3455,11 @@
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
     </row>
-    <row r="43" spans="5:16">
+    <row r="43" spans="1:16">
       <c r="E43" s="7"/>
       <c r="F43" s="8"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="24"/>
+      <c r="H43" s="23"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -3051,11 +3469,11 @@
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
     </row>
-    <row r="44" spans="5:16">
+    <row r="44" spans="1:16">
       <c r="E44" s="7"/>
       <c r="F44" s="8"/>
       <c r="G44" s="7"/>
-      <c r="H44" s="24"/>
+      <c r="H44" s="23"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
@@ -3065,11 +3483,11 @@
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
     </row>
-    <row r="45" spans="5:16">
+    <row r="45" spans="1:16">
       <c r="E45" s="7"/>
       <c r="F45" s="8"/>
       <c r="G45" s="7"/>
-      <c r="H45" s="24"/>
+      <c r="H45" s="23"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
@@ -3079,11 +3497,11 @@
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
     </row>
-    <row r="46" spans="5:16">
+    <row r="46" spans="1:16">
       <c r="E46" s="7"/>
       <c r="F46" s="8"/>
       <c r="G46" s="7"/>
-      <c r="H46" s="24"/>
+      <c r="H46" s="23"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
@@ -3093,11 +3511,11 @@
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
     </row>
-    <row r="47" spans="5:16">
+    <row r="47" spans="1:16">
       <c r="E47" s="7"/>
       <c r="F47" s="8"/>
       <c r="G47" s="7"/>
-      <c r="H47" s="24"/>
+      <c r="H47" s="23"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
@@ -3107,11 +3525,11 @@
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
     </row>
-    <row r="48" spans="5:16">
+    <row r="48" spans="1:16">
       <c r="E48" s="7"/>
       <c r="F48" s="8"/>
       <c r="G48" s="7"/>
-      <c r="H48" s="24"/>
+      <c r="H48" s="23"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
@@ -3125,7 +3543,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="8"/>
       <c r="G49" s="7"/>
-      <c r="H49" s="24"/>
+      <c r="H49" s="23"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
@@ -3139,7 +3557,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="8"/>
       <c r="G50" s="7"/>
-      <c r="H50" s="24"/>
+      <c r="H50" s="23"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
@@ -3153,7 +3571,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="8"/>
       <c r="G51" s="7"/>
-      <c r="H51" s="24"/>
+      <c r="H51" s="23"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
@@ -3167,7 +3585,7 @@
       <c r="E52" s="7"/>
       <c r="F52" s="8"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="24"/>
+      <c r="H52" s="23"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
@@ -3181,7 +3599,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="8"/>
       <c r="G53" s="7"/>
-      <c r="H53" s="24"/>
+      <c r="H53" s="23"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
@@ -3195,7 +3613,7 @@
       <c r="E54" s="7"/>
       <c r="F54" s="8"/>
       <c r="G54" s="7"/>
-      <c r="H54" s="24"/>
+      <c r="H54" s="23"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
@@ -3209,7 +3627,7 @@
       <c r="E55" s="7"/>
       <c r="F55" s="8"/>
       <c r="G55" s="7"/>
-      <c r="H55" s="24"/>
+      <c r="H55" s="23"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
       <c r="K55" s="7"/>
@@ -3223,7 +3641,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="8"/>
       <c r="G56" s="7"/>
-      <c r="H56" s="24"/>
+      <c r="H56" s="23"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="7"/>
@@ -3237,7 +3655,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="8"/>
       <c r="G57" s="7"/>
-      <c r="H57" s="24"/>
+      <c r="H57" s="23"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="7"/>
@@ -3251,7 +3669,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="8"/>
       <c r="G58" s="7"/>
-      <c r="H58" s="24"/>
+      <c r="H58" s="23"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="7"/>
@@ -3265,7 +3683,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="8"/>
       <c r="G59" s="7"/>
-      <c r="H59" s="24"/>
+      <c r="H59" s="23"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="7"/>
@@ -3279,7 +3697,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="8"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="24"/>
+      <c r="H60" s="23"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
@@ -3293,7 +3711,7 @@
       <c r="E61" s="7"/>
       <c r="F61" s="8"/>
       <c r="G61" s="7"/>
-      <c r="H61" s="24"/>
+      <c r="H61" s="23"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
       <c r="K61" s="7"/>
@@ -3307,7 +3725,7 @@
       <c r="E62" s="7"/>
       <c r="F62" s="8"/>
       <c r="G62" s="7"/>
-      <c r="H62" s="24"/>
+      <c r="H62" s="23"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
       <c r="K62" s="7"/>
@@ -3321,7 +3739,7 @@
       <c r="E63" s="7"/>
       <c r="F63" s="8"/>
       <c r="G63" s="7"/>
-      <c r="H63" s="24"/>
+      <c r="H63" s="23"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
       <c r="K63" s="7"/>
@@ -3335,7 +3753,7 @@
       <c r="E64" s="7"/>
       <c r="F64" s="8"/>
       <c r="G64" s="7"/>
-      <c r="H64" s="24"/>
+      <c r="H64" s="23"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
       <c r="K64" s="7"/>
@@ -3349,7 +3767,7 @@
       <c r="E65" s="7"/>
       <c r="F65" s="8"/>
       <c r="G65" s="7"/>
-      <c r="H65" s="24"/>
+      <c r="H65" s="23"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
@@ -3363,7 +3781,7 @@
       <c r="E66" s="7"/>
       <c r="F66" s="8"/>
       <c r="G66" s="7"/>
-      <c r="H66" s="24"/>
+      <c r="H66" s="23"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
       <c r="K66" s="7"/>
@@ -3377,7 +3795,7 @@
       <c r="E67" s="7"/>
       <c r="F67" s="8"/>
       <c r="G67" s="7"/>
-      <c r="H67" s="24"/>
+      <c r="H67" s="23"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
       <c r="K67" s="7"/>
@@ -3391,7 +3809,7 @@
       <c r="E68" s="7"/>
       <c r="F68" s="8"/>
       <c r="G68" s="7"/>
-      <c r="H68" s="24"/>
+      <c r="H68" s="23"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
       <c r="K68" s="7"/>
@@ -3405,7 +3823,7 @@
       <c r="E69" s="7"/>
       <c r="F69" s="8"/>
       <c r="G69" s="7"/>
-      <c r="H69" s="24"/>
+      <c r="H69" s="23"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
       <c r="K69" s="7"/>
@@ -3419,7 +3837,7 @@
       <c r="E70" s="7"/>
       <c r="F70" s="8"/>
       <c r="G70" s="7"/>
-      <c r="H70" s="24"/>
+      <c r="H70" s="23"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
       <c r="K70" s="7"/>
@@ -3433,7 +3851,7 @@
       <c r="E71" s="7"/>
       <c r="F71" s="8"/>
       <c r="G71" s="7"/>
-      <c r="H71" s="24"/>
+      <c r="H71" s="23"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
       <c r="K71" s="7"/>
@@ -3447,7 +3865,7 @@
       <c r="E72" s="7"/>
       <c r="F72" s="8"/>
       <c r="G72" s="7"/>
-      <c r="H72" s="24"/>
+      <c r="H72" s="23"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
       <c r="K72" s="7"/>
@@ -3461,7 +3879,7 @@
       <c r="E73" s="7"/>
       <c r="F73" s="8"/>
       <c r="G73" s="7"/>
-      <c r="H73" s="24"/>
+      <c r="H73" s="23"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
       <c r="K73" s="7"/>
@@ -3475,7 +3893,7 @@
       <c r="E74" s="7"/>
       <c r="F74" s="8"/>
       <c r="G74" s="7"/>
-      <c r="H74" s="24"/>
+      <c r="H74" s="23"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
       <c r="K74" s="7"/>
@@ -3489,7 +3907,7 @@
       <c r="E75" s="7"/>
       <c r="F75" s="8"/>
       <c r="G75" s="7"/>
-      <c r="H75" s="24"/>
+      <c r="H75" s="23"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
       <c r="K75" s="7"/>
@@ -3503,7 +3921,7 @@
       <c r="E76" s="7"/>
       <c r="F76" s="8"/>
       <c r="G76" s="7"/>
-      <c r="H76" s="24"/>
+      <c r="H76" s="23"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
       <c r="K76" s="7"/>
@@ -3517,7 +3935,7 @@
       <c r="E77" s="7"/>
       <c r="F77" s="8"/>
       <c r="G77" s="7"/>
-      <c r="H77" s="24"/>
+      <c r="H77" s="23"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
       <c r="K77" s="7"/>
@@ -3531,7 +3949,7 @@
       <c r="E78" s="7"/>
       <c r="F78" s="8"/>
       <c r="G78" s="7"/>
-      <c r="H78" s="24"/>
+      <c r="H78" s="23"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
       <c r="K78" s="7"/>
@@ -3545,7 +3963,7 @@
       <c r="E79" s="7"/>
       <c r="F79" s="8"/>
       <c r="G79" s="7"/>
-      <c r="H79" s="24"/>
+      <c r="H79" s="23"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
       <c r="K79" s="7"/>
@@ -3559,7 +3977,7 @@
       <c r="E80" s="7"/>
       <c r="F80" s="8"/>
       <c r="G80" s="7"/>
-      <c r="H80" s="24"/>
+      <c r="H80" s="23"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
       <c r="K80" s="7"/>
@@ -3573,7 +3991,7 @@
       <c r="E81" s="7"/>
       <c r="F81" s="8"/>
       <c r="G81" s="7"/>
-      <c r="H81" s="24"/>
+      <c r="H81" s="23"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -3587,7 +4005,7 @@
       <c r="E82" s="7"/>
       <c r="F82" s="8"/>
       <c r="G82" s="7"/>
-      <c r="H82" s="24"/>
+      <c r="H82" s="23"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
       <c r="K82" s="7"/>
@@ -3601,7 +4019,7 @@
       <c r="E83" s="7"/>
       <c r="F83" s="8"/>
       <c r="G83" s="7"/>
-      <c r="H83" s="24"/>
+      <c r="H83" s="23"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
       <c r="K83" s="7"/>
@@ -3615,7 +4033,7 @@
       <c r="E84" s="7"/>
       <c r="F84" s="8"/>
       <c r="G84" s="7"/>
-      <c r="H84" s="24"/>
+      <c r="H84" s="23"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
       <c r="K84" s="7"/>
@@ -3629,7 +4047,7 @@
       <c r="E85" s="7"/>
       <c r="F85" s="8"/>
       <c r="G85" s="7"/>
-      <c r="H85" s="24"/>
+      <c r="H85" s="23"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
       <c r="K85" s="7"/>
@@ -3643,7 +4061,7 @@
       <c r="E86" s="7"/>
       <c r="F86" s="8"/>
       <c r="G86" s="7"/>
-      <c r="H86" s="24"/>
+      <c r="H86" s="23"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
       <c r="K86" s="7"/>
@@ -3657,7 +4075,7 @@
       <c r="E87" s="7"/>
       <c r="F87" s="8"/>
       <c r="G87" s="7"/>
-      <c r="H87" s="24"/>
+      <c r="H87" s="23"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
       <c r="K87" s="7"/>
@@ -3671,7 +4089,7 @@
       <c r="E88" s="7"/>
       <c r="F88" s="8"/>
       <c r="G88" s="7"/>
-      <c r="H88" s="24"/>
+      <c r="H88" s="23"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
       <c r="K88" s="7"/>
@@ -3685,7 +4103,7 @@
       <c r="E89" s="7"/>
       <c r="F89" s="8"/>
       <c r="G89" s="7"/>
-      <c r="H89" s="24"/>
+      <c r="H89" s="23"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
       <c r="K89" s="7"/>
@@ -3699,7 +4117,7 @@
       <c r="E90" s="7"/>
       <c r="F90" s="8"/>
       <c r="G90" s="7"/>
-      <c r="H90" s="24"/>
+      <c r="H90" s="23"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
       <c r="K90" s="7"/>
@@ -3713,7 +4131,7 @@
       <c r="E91" s="7"/>
       <c r="F91" s="8"/>
       <c r="G91" s="7"/>
-      <c r="H91" s="24"/>
+      <c r="H91" s="23"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
       <c r="K91" s="7"/>
@@ -3727,7 +4145,7 @@
       <c r="E92" s="7"/>
       <c r="F92" s="8"/>
       <c r="G92" s="7"/>
-      <c r="H92" s="24"/>
+      <c r="H92" s="23"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
       <c r="K92" s="7"/>
@@ -3741,7 +4159,7 @@
       <c r="E93" s="7"/>
       <c r="F93" s="8"/>
       <c r="G93" s="7"/>
-      <c r="H93" s="24"/>
+      <c r="H93" s="23"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
       <c r="K93" s="7"/>
@@ -3755,7 +4173,7 @@
       <c r="E94" s="7"/>
       <c r="F94" s="8"/>
       <c r="G94" s="7"/>
-      <c r="H94" s="24"/>
+      <c r="H94" s="23"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
       <c r="K94" s="7"/>
@@ -3769,7 +4187,7 @@
       <c r="E95" s="7"/>
       <c r="F95" s="8"/>
       <c r="G95" s="7"/>
-      <c r="H95" s="24"/>
+      <c r="H95" s="23"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
       <c r="K95" s="7"/>
@@ -3783,7 +4201,7 @@
       <c r="E96" s="7"/>
       <c r="F96" s="8"/>
       <c r="G96" s="7"/>
-      <c r="H96" s="24"/>
+      <c r="H96" s="23"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
       <c r="K96" s="7"/>
@@ -3797,7 +4215,7 @@
       <c r="E97" s="7"/>
       <c r="F97" s="8"/>
       <c r="G97" s="7"/>
-      <c r="H97" s="24"/>
+      <c r="H97" s="23"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
       <c r="K97" s="7"/>
@@ -3811,7 +4229,7 @@
       <c r="E98" s="7"/>
       <c r="F98" s="8"/>
       <c r="G98" s="7"/>
-      <c r="H98" s="24"/>
+      <c r="H98" s="23"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
@@ -3825,7 +4243,7 @@
       <c r="E99" s="7"/>
       <c r="F99" s="8"/>
       <c r="G99" s="7"/>
-      <c r="H99" s="24"/>
+      <c r="H99" s="23"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
       <c r="K99" s="7"/>
@@ -3839,7 +4257,7 @@
       <c r="E100" s="7"/>
       <c r="F100" s="8"/>
       <c r="G100" s="7"/>
-      <c r="H100" s="24"/>
+      <c r="H100" s="23"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
       <c r="K100" s="7"/>
@@ -3853,7 +4271,7 @@
       <c r="E101" s="7"/>
       <c r="F101" s="8"/>
       <c r="G101" s="7"/>
-      <c r="H101" s="24"/>
+      <c r="H101" s="23"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
       <c r="K101" s="7"/>
@@ -3867,7 +4285,7 @@
       <c r="E102" s="7"/>
       <c r="F102" s="8"/>
       <c r="G102" s="7"/>
-      <c r="H102" s="24"/>
+      <c r="H102" s="23"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
       <c r="K102" s="7"/>
@@ -3881,7 +4299,7 @@
       <c r="E103" s="7"/>
       <c r="F103" s="8"/>
       <c r="G103" s="7"/>
-      <c r="H103" s="24"/>
+      <c r="H103" s="23"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
       <c r="K103" s="7"/>
@@ -3895,7 +4313,7 @@
       <c r="E104" s="7"/>
       <c r="F104" s="8"/>
       <c r="G104" s="7"/>
-      <c r="H104" s="24"/>
+      <c r="H104" s="23"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
       <c r="K104" s="7"/>
@@ -3909,7 +4327,7 @@
       <c r="E105" s="7"/>
       <c r="F105" s="8"/>
       <c r="G105" s="7"/>
-      <c r="H105" s="24"/>
+      <c r="H105" s="23"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
@@ -3923,7 +4341,7 @@
       <c r="E106" s="7"/>
       <c r="F106" s="8"/>
       <c r="G106" s="7"/>
-      <c r="H106" s="24"/>
+      <c r="H106" s="23"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
@@ -3937,7 +4355,7 @@
       <c r="E107" s="7"/>
       <c r="F107" s="8"/>
       <c r="G107" s="7"/>
-      <c r="H107" s="24"/>
+      <c r="H107" s="23"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
@@ -3951,7 +4369,7 @@
       <c r="E108" s="7"/>
       <c r="F108" s="8"/>
       <c r="G108" s="7"/>
-      <c r="H108" s="24"/>
+      <c r="H108" s="23"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
       <c r="K108" s="7"/>
@@ -3965,7 +4383,7 @@
       <c r="E109" s="7"/>
       <c r="F109" s="8"/>
       <c r="G109" s="7"/>
-      <c r="H109" s="24"/>
+      <c r="H109" s="23"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
@@ -3979,7 +4397,7 @@
       <c r="E110" s="7"/>
       <c r="F110" s="8"/>
       <c r="G110" s="7"/>
-      <c r="H110" s="24"/>
+      <c r="H110" s="23"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
       <c r="K110" s="7"/>
@@ -3993,7 +4411,7 @@
       <c r="E111" s="7"/>
       <c r="F111" s="8"/>
       <c r="G111" s="7"/>
-      <c r="H111" s="24"/>
+      <c r="H111" s="23"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
       <c r="K111" s="7"/>
@@ -4007,7 +4425,7 @@
       <c r="E112" s="7"/>
       <c r="F112" s="8"/>
       <c r="G112" s="7"/>
-      <c r="H112" s="24"/>
+      <c r="H112" s="23"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
       <c r="K112" s="7"/>
@@ -4021,7 +4439,7 @@
       <c r="E113" s="7"/>
       <c r="F113" s="8"/>
       <c r="G113" s="7"/>
-      <c r="H113" s="24"/>
+      <c r="H113" s="23"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
       <c r="K113" s="7"/>
@@ -4035,7 +4453,7 @@
       <c r="E114" s="7"/>
       <c r="F114" s="8"/>
       <c r="G114" s="7"/>
-      <c r="H114" s="24"/>
+      <c r="H114" s="23"/>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
       <c r="K114" s="7"/>
@@ -4049,7 +4467,7 @@
       <c r="E115" s="7"/>
       <c r="F115" s="8"/>
       <c r="G115" s="7"/>
-      <c r="H115" s="24"/>
+      <c r="H115" s="23"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
       <c r="K115" s="7"/>
@@ -4063,7 +4481,7 @@
       <c r="E116" s="7"/>
       <c r="F116" s="8"/>
       <c r="G116" s="7"/>
-      <c r="H116" s="24"/>
+      <c r="H116" s="23"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
       <c r="K116" s="7"/>
@@ -4077,7 +4495,7 @@
       <c r="E117" s="7"/>
       <c r="F117" s="8"/>
       <c r="G117" s="7"/>
-      <c r="H117" s="24"/>
+      <c r="H117" s="23"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
       <c r="K117" s="7"/>
@@ -4091,7 +4509,7 @@
       <c r="E118" s="7"/>
       <c r="F118" s="8"/>
       <c r="G118" s="7"/>
-      <c r="H118" s="24"/>
+      <c r="H118" s="23"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
       <c r="K118" s="7"/>
@@ -4105,7 +4523,7 @@
       <c r="E119" s="7"/>
       <c r="F119" s="8"/>
       <c r="G119" s="7"/>
-      <c r="H119" s="24"/>
+      <c r="H119" s="23"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
       <c r="K119" s="7"/>
@@ -4119,7 +4537,7 @@
       <c r="E120" s="7"/>
       <c r="F120" s="8"/>
       <c r="G120" s="7"/>
-      <c r="H120" s="24"/>
+      <c r="H120" s="23"/>
       <c r="I120" s="7"/>
       <c r="J120" s="7"/>
       <c r="K120" s="7"/>
@@ -4133,7 +4551,7 @@
       <c r="E121" s="7"/>
       <c r="F121" s="8"/>
       <c r="G121" s="7"/>
-      <c r="H121" s="24"/>
+      <c r="H121" s="23"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
       <c r="K121" s="7"/>
@@ -4147,7 +4565,7 @@
       <c r="E122" s="7"/>
       <c r="F122" s="8"/>
       <c r="G122" s="7"/>
-      <c r="H122" s="24"/>
+      <c r="H122" s="23"/>
       <c r="I122" s="7"/>
       <c r="J122" s="7"/>
       <c r="K122" s="7"/>
@@ -4161,7 +4579,7 @@
       <c r="E123" s="7"/>
       <c r="F123" s="8"/>
       <c r="G123" s="7"/>
-      <c r="H123" s="24"/>
+      <c r="H123" s="23"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
       <c r="K123" s="7"/>
@@ -4175,7 +4593,7 @@
       <c r="E124" s="7"/>
       <c r="F124" s="8"/>
       <c r="G124" s="7"/>
-      <c r="H124" s="24"/>
+      <c r="H124" s="23"/>
       <c r="I124" s="7"/>
       <c r="J124" s="7"/>
       <c r="K124" s="7"/>
@@ -4189,7 +4607,7 @@
       <c r="E125" s="7"/>
       <c r="F125" s="8"/>
       <c r="G125" s="7"/>
-      <c r="H125" s="24"/>
+      <c r="H125" s="23"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
       <c r="K125" s="7"/>
@@ -4203,7 +4621,7 @@
       <c r="E126" s="7"/>
       <c r="F126" s="8"/>
       <c r="G126" s="7"/>
-      <c r="H126" s="24"/>
+      <c r="H126" s="23"/>
       <c r="I126" s="7"/>
       <c r="J126" s="7"/>
       <c r="K126" s="7"/>
@@ -4217,7 +4635,7 @@
       <c r="E127" s="7"/>
       <c r="F127" s="8"/>
       <c r="G127" s="7"/>
-      <c r="H127" s="24"/>
+      <c r="H127" s="23"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
       <c r="K127" s="7"/>
@@ -4231,7 +4649,7 @@
       <c r="E128" s="7"/>
       <c r="F128" s="8"/>
       <c r="G128" s="7"/>
-      <c r="H128" s="24"/>
+      <c r="H128" s="23"/>
       <c r="I128" s="7"/>
       <c r="J128" s="7"/>
       <c r="K128" s="7"/>
@@ -4245,7 +4663,7 @@
       <c r="E129" s="7"/>
       <c r="F129" s="8"/>
       <c r="G129" s="7"/>
-      <c r="H129" s="24"/>
+      <c r="H129" s="23"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
       <c r="K129" s="7"/>
@@ -4259,7 +4677,7 @@
       <c r="E130" s="7"/>
       <c r="F130" s="8"/>
       <c r="G130" s="7"/>
-      <c r="H130" s="24"/>
+      <c r="H130" s="23"/>
       <c r="I130" s="7"/>
       <c r="J130" s="7"/>
       <c r="K130" s="7"/>
@@ -4273,7 +4691,7 @@
       <c r="E131" s="7"/>
       <c r="F131" s="8"/>
       <c r="G131" s="7"/>
-      <c r="H131" s="24"/>
+      <c r="H131" s="23"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
       <c r="K131" s="7"/>
@@ -4287,7 +4705,7 @@
       <c r="E132" s="7"/>
       <c r="F132" s="8"/>
       <c r="G132" s="7"/>
-      <c r="H132" s="24"/>
+      <c r="H132" s="23"/>
       <c r="I132" s="7"/>
       <c r="J132" s="7"/>
       <c r="K132" s="7"/>
@@ -4301,7 +4719,7 @@
       <c r="E133" s="7"/>
       <c r="F133" s="8"/>
       <c r="G133" s="7"/>
-      <c r="H133" s="24"/>
+      <c r="H133" s="23"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
       <c r="K133" s="7"/>
@@ -4315,7 +4733,7 @@
       <c r="E134" s="7"/>
       <c r="F134" s="8"/>
       <c r="G134" s="7"/>
-      <c r="H134" s="24"/>
+      <c r="H134" s="23"/>
       <c r="I134" s="7"/>
       <c r="J134" s="7"/>
       <c r="K134" s="7"/>
@@ -4329,7 +4747,7 @@
       <c r="E135" s="7"/>
       <c r="F135" s="8"/>
       <c r="G135" s="7"/>
-      <c r="H135" s="24"/>
+      <c r="H135" s="23"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
       <c r="K135" s="7"/>
@@ -4343,7 +4761,7 @@
       <c r="E136" s="7"/>
       <c r="F136" s="8"/>
       <c r="G136" s="7"/>
-      <c r="H136" s="24"/>
+      <c r="H136" s="23"/>
       <c r="I136" s="7"/>
       <c r="J136" s="7"/>
       <c r="K136" s="7"/>
@@ -4357,7 +4775,7 @@
       <c r="E137" s="7"/>
       <c r="F137" s="8"/>
       <c r="G137" s="7"/>
-      <c r="H137" s="24"/>
+      <c r="H137" s="23"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
       <c r="K137" s="7"/>
@@ -4371,7 +4789,7 @@
       <c r="E138" s="7"/>
       <c r="F138" s="8"/>
       <c r="G138" s="7"/>
-      <c r="H138" s="24"/>
+      <c r="H138" s="23"/>
       <c r="I138" s="7"/>
       <c r="J138" s="7"/>
       <c r="K138" s="7"/>
@@ -4385,7 +4803,7 @@
       <c r="E139" s="7"/>
       <c r="F139" s="8"/>
       <c r="G139" s="7"/>
-      <c r="H139" s="24"/>
+      <c r="H139" s="23"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
       <c r="K139" s="7"/>
@@ -4399,7 +4817,7 @@
       <c r="E140" s="7"/>
       <c r="F140" s="8"/>
       <c r="G140" s="7"/>
-      <c r="H140" s="24"/>
+      <c r="H140" s="23"/>
       <c r="I140" s="7"/>
       <c r="J140" s="7"/>
       <c r="K140" s="7"/>
@@ -4413,7 +4831,7 @@
       <c r="E141" s="7"/>
       <c r="F141" s="8"/>
       <c r="G141" s="7"/>
-      <c r="H141" s="24"/>
+      <c r="H141" s="23"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
       <c r="K141" s="7"/>
@@ -4427,7 +4845,7 @@
       <c r="E142" s="7"/>
       <c r="F142" s="8"/>
       <c r="G142" s="7"/>
-      <c r="H142" s="24"/>
+      <c r="H142" s="23"/>
       <c r="I142" s="7"/>
       <c r="J142" s="7"/>
       <c r="K142" s="7"/>
@@ -4441,7 +4859,7 @@
       <c r="E143" s="7"/>
       <c r="F143" s="8"/>
       <c r="G143" s="7"/>
-      <c r="H143" s="24"/>
+      <c r="H143" s="23"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
       <c r="K143" s="7"/>
@@ -4455,7 +4873,7 @@
       <c r="E144" s="7"/>
       <c r="F144" s="8"/>
       <c r="G144" s="7"/>
-      <c r="H144" s="24"/>
+      <c r="H144" s="23"/>
       <c r="I144" s="7"/>
       <c r="J144" s="7"/>
       <c r="K144" s="7"/>
@@ -4469,7 +4887,7 @@
       <c r="E145" s="7"/>
       <c r="F145" s="8"/>
       <c r="G145" s="7"/>
-      <c r="H145" s="24"/>
+      <c r="H145" s="23"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
       <c r="K145" s="7"/>
@@ -4483,7 +4901,7 @@
       <c r="E146" s="7"/>
       <c r="F146" s="8"/>
       <c r="G146" s="7"/>
-      <c r="H146" s="24"/>
+      <c r="H146" s="23"/>
       <c r="I146" s="7"/>
       <c r="J146" s="7"/>
       <c r="K146" s="7"/>
@@ -4497,7 +4915,7 @@
       <c r="E147" s="7"/>
       <c r="F147" s="8"/>
       <c r="G147" s="7"/>
-      <c r="H147" s="24"/>
+      <c r="H147" s="23"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
       <c r="K147" s="7"/>
@@ -4511,7 +4929,7 @@
       <c r="E148" s="7"/>
       <c r="F148" s="8"/>
       <c r="G148" s="7"/>
-      <c r="H148" s="24"/>
+      <c r="H148" s="23"/>
       <c r="I148" s="7"/>
       <c r="J148" s="7"/>
       <c r="K148" s="7"/>
@@ -4525,7 +4943,7 @@
       <c r="E149" s="7"/>
       <c r="F149" s="8"/>
       <c r="G149" s="7"/>
-      <c r="H149" s="24"/>
+      <c r="H149" s="23"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
       <c r="K149" s="7"/>
@@ -4539,7 +4957,7 @@
       <c r="E150" s="7"/>
       <c r="F150" s="8"/>
       <c r="G150" s="7"/>
-      <c r="H150" s="24"/>
+      <c r="H150" s="23"/>
       <c r="I150" s="7"/>
       <c r="J150" s="7"/>
       <c r="K150" s="7"/>
@@ -4553,7 +4971,7 @@
       <c r="E151" s="7"/>
       <c r="F151" s="8"/>
       <c r="G151" s="7"/>
-      <c r="H151" s="24"/>
+      <c r="H151" s="23"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
       <c r="K151" s="7"/>
@@ -4567,7 +4985,7 @@
       <c r="E152" s="7"/>
       <c r="F152" s="8"/>
       <c r="G152" s="7"/>
-      <c r="H152" s="24"/>
+      <c r="H152" s="23"/>
       <c r="I152" s="7"/>
       <c r="J152" s="7"/>
       <c r="K152" s="7"/>
@@ -4581,7 +4999,7 @@
       <c r="E153" s="7"/>
       <c r="F153" s="8"/>
       <c r="G153" s="7"/>
-      <c r="H153" s="24"/>
+      <c r="H153" s="23"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
       <c r="K153" s="7"/>
@@ -4595,7 +5013,7 @@
       <c r="E154" s="7"/>
       <c r="F154" s="8"/>
       <c r="G154" s="7"/>
-      <c r="H154" s="24"/>
+      <c r="H154" s="23"/>
       <c r="I154" s="7"/>
       <c r="J154" s="7"/>
       <c r="K154" s="7"/>
@@ -4609,7 +5027,7 @@
       <c r="E155" s="7"/>
       <c r="F155" s="8"/>
       <c r="G155" s="7"/>
-      <c r="H155" s="24"/>
+      <c r="H155" s="23"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
       <c r="K155" s="7"/>
@@ -4623,7 +5041,7 @@
       <c r="E156" s="7"/>
       <c r="F156" s="8"/>
       <c r="G156" s="7"/>
-      <c r="H156" s="24"/>
+      <c r="H156" s="23"/>
       <c r="I156" s="7"/>
       <c r="J156" s="7"/>
       <c r="K156" s="7"/>
@@ -4637,7 +5055,7 @@
       <c r="E157" s="7"/>
       <c r="F157" s="8"/>
       <c r="G157" s="7"/>
-      <c r="H157" s="24"/>
+      <c r="H157" s="23"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
       <c r="K157" s="7"/>
@@ -4651,7 +5069,7 @@
       <c r="E158" s="7"/>
       <c r="F158" s="8"/>
       <c r="G158" s="7"/>
-      <c r="H158" s="7"/>
+      <c r="H158" s="23"/>
       <c r="I158" s="7"/>
       <c r="J158" s="7"/>
       <c r="K158" s="7"/>
@@ -4665,7 +5083,7 @@
       <c r="E159" s="7"/>
       <c r="F159" s="8"/>
       <c r="G159" s="7"/>
-      <c r="H159" s="7"/>
+      <c r="H159" s="23"/>
       <c r="I159" s="7"/>
       <c r="J159" s="7"/>
       <c r="K159" s="7"/>
@@ -4677,7 +5095,7 @@
     </row>
     <row r="160" spans="5:16">
       <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
+      <c r="F160" s="8"/>
       <c r="G160" s="7"/>
       <c r="H160" s="7"/>
       <c r="I160" s="7"/>
@@ -4691,7 +5109,7 @@
     </row>
     <row r="161" spans="5:16">
       <c r="E161" s="7"/>
-      <c r="F161" s="7"/>
+      <c r="F161" s="8"/>
       <c r="G161" s="7"/>
       <c r="H161" s="7"/>
       <c r="I161" s="7"/>
@@ -4703,16 +5121,54 @@
       <c r="O161" s="7"/>
       <c r="P161" s="7"/>
     </row>
+    <row r="162" spans="5:16">
+      <c r="E162" s="7"/>
+      <c r="F162" s="7"/>
+      <c r="G162" s="7"/>
+      <c r="H162" s="7"/>
+      <c r="I162" s="7"/>
+      <c r="J162" s="7"/>
+      <c r="K162" s="7"/>
+      <c r="L162" s="7"/>
+      <c r="M162" s="7"/>
+      <c r="N162" s="7"/>
+      <c r="O162" s="7"/>
+      <c r="P162" s="7"/>
+    </row>
+    <row r="163" spans="5:16">
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
+      <c r="H163" s="7"/>
+      <c r="I163" s="7"/>
+      <c r="J163" s="7"/>
+      <c r="K163" s="7"/>
+      <c r="L163" s="7"/>
+      <c r="M163" s="7"/>
+      <c r="N163" s="7"/>
+      <c r="O163" s="7"/>
+      <c r="P163" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H44:H159">
+  <conditionalFormatting sqref="H46:H161">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Passed ">
-      <formula>NOT(ISERROR(SEARCH("Passed ",H44)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Passed ",H46)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D14" r:id="rId2" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D15" r:id="rId3" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D16" r:id="rId4" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D13" r:id="rId5" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D25" r:id="rId6" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D6" r:id="rId7" display="cmcclune02@qub.ac.uk"/>
+    <hyperlink ref="D5" r:id="rId8" display="cmcclune02@qub.ac.uk"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -4720,25 +5176,25 @@
           <x14:formula1>
             <xm:f>Settings!$A$4:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H43</xm:sqref>
+          <xm:sqref>H2:H45</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F159</xm:sqref>
+          <xm:sqref>F2:F161</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$F$4:$F$8</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L7</xm:sqref>
+          <xm:sqref>L2:L9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K11</xm:sqref>
+          <xm:sqref>K2:K13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4756,8 +5212,8 @@
   </sheetPr>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4771,19 +5227,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F1" s="1"/>
@@ -4797,11 +5253,14 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" ht="23">
-      <c r="A2" t="s">
-        <v>64</v>
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="F2" s="1"/>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>52</v>
       </c>
       <c r="I2" s="1"/>
@@ -4812,7 +5271,9 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="B3" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -4827,7 +5288,9 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="B4" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -4842,7 +5305,9 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="B5" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -4857,7 +5322,9 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -4872,7 +5339,9 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -4887,7 +5356,9 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -4902,7 +5373,9 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -4917,7 +5390,9 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -4932,7 +5407,9 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="3" t="s">
+        <v>133</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -4947,7 +5424,9 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -4962,7 +5441,9 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>135</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -4977,7 +5458,9 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -4992,7 +5475,9 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="3" t="s">
+        <v>137</v>
+      </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -5007,7 +5492,9 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -5022,7 +5509,9 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="3" t="s">
+        <v>139</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5037,7 +5526,9 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5052,7 +5543,9 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>141</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -5065,22 +5558,41 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
     </row>
-    <row r="32" spans="1:13" ht="28">
-      <c r="A32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>63</v>
-      </c>
+    <row r="20" spans="1:13">
+      <c r="B20" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="B21" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="B22" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="B23" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="B25" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5123,7 +5635,7 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B4" t="s">
@@ -5137,7 +5649,7 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
@@ -5151,7 +5663,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
@@ -5185,12 +5697,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -5304,7 +5810,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5313,16 +5819,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5338,10 +5841,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>